<commit_message>
Upgraded codebase to allow global variables to be passed in a packed argument called globvars that is just a package of kwargs.
</commit_message>
<xml_diff>
--- a/REACTION_NETWORK.xlsx
+++ b/REACTION_NETWORK.xlsx
@@ -23,9 +23,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6098" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6099" uniqueCount="399">
   <si>
-    <t xml:space="preserve">No</t>
+    <t xml:space="preserve">Num</t>
   </si>
   <si>
     <t xml:space="preserve">R1</t>
@@ -1231,7 +1231,7 @@
     <numFmt numFmtId="165" formatCode="General"/>
     <numFmt numFmtId="166" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1252,11 +1252,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1301,7 +1296,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1322,15 +1317,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1356,10 +1343,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A290" activeCellId="0" sqref="A290"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.79"/>
@@ -18549,12 +18536,12 @@
   <dimension ref="A1:Y678"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I89" activeCellId="0" sqref="I89"/>
+      <selection pane="bottomLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.52"/>
@@ -18578,7 +18565,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
@@ -23744,7 +23731,7 @@
         <v>Yelle</v>
       </c>
     </row>
-    <row r="88" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="4" t="n">
         <f aca="false">ROW()-1</f>
         <v>87</v>
@@ -23772,7 +23759,7 @@
       <c r="L88" s="5" t="n">
         <v>2.24E-009</v>
       </c>
-      <c r="M88" s="6" t="n">
+      <c r="M88" s="1" t="n">
         <v>-0.15</v>
       </c>
       <c r="N88" s="4" t="n">
@@ -59832,7 +59819,7 @@
       <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.65"/>
@@ -61794,7 +61781,7 @@
       <selection pane="topLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">

</xml_diff>

<commit_message>
Updated code base to load photodissociation and photoionization reactions from a file, automatically build J rate symbols.
</commit_message>
<xml_diff>
--- a/REACTION_NETWORK.xlsx
+++ b/REACTION_NETWORK.xlsx
@@ -5,13 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Neutral reactions" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Ion reactions" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Unused neutrals" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Unused ion reactions" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Photodissociation" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Photoionization" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Unused neutrals" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Unused ion reactions" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6283" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6550" uniqueCount="411">
   <si>
     <t xml:space="preserve">Num</t>
   </si>
@@ -1165,6 +1167,27 @@
     <t xml:space="preserve">LeGarrec03</t>
   </si>
   <si>
+    <t xml:space="preserve">J</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2OH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2plpl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cplpl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Missing D analogue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2O2pl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O3pl</t>
+  </si>
+  <si>
     <t xml:space="preserve">I believe these are all here because we already had the reaction so I just used the one we already had + whatever rate seemed best</t>
   </si>
   <si>
@@ -1269,12 +1292,18 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1311,7 +1340,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1328,11 +1357,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1358,10 +1391,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A173" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.79"/>
@@ -18550,11 +18583,11 @@
   </sheetPr>
   <dimension ref="A1:AA678"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.52"/>
@@ -18563,7 +18596,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="3.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="4.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="4.63"/>
@@ -18576,7 +18609,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="5.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="24.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="27.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="27.46"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24167,68 +24200,68 @@
         <f aca="false">ROW()-2</f>
         <v>92</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B94" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="C94" s="4" t="s">
+      <c r="C94" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D94" s="4" t="s">
+      <c r="D94" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="E94" s="4" t="s">
+      <c r="E94" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F94" s="4"/>
-      <c r="G94" s="4" t="n">
+      <c r="F94" s="1"/>
+      <c r="G94" s="1" t="n">
         <v>-2</v>
       </c>
-      <c r="H94" s="4" t="s">
+      <c r="H94" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="I94" s="4"/>
-      <c r="J94" s="4"/>
-      <c r="K94" s="4"/>
-      <c r="L94" s="4"/>
-      <c r="M94" s="4"/>
-      <c r="N94" s="5" t="n">
+      <c r="I94" s="1"/>
+      <c r="J94" s="1"/>
+      <c r="K94" s="1"/>
+      <c r="L94" s="1"/>
+      <c r="M94" s="1"/>
+      <c r="N94" s="4" t="n">
         <v>2.24E-009</v>
       </c>
       <c r="O94" s="1" t="n">
         <v>-0.15</v>
       </c>
-      <c r="P94" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q94" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R94" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="S94" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="T94" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="U94" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="V94" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="W94" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="X94" s="4" t="s">
+      <c r="P94" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q94" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R94" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S94" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T94" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U94" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V94" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W94" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X94" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="Y94" s="4" t="s">
+      <c r="Y94" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="Z94" s="4"/>
-      <c r="AA94" s="4" t="str">
+      <c r="Z94" s="1"/>
+      <c r="AA94" s="1" t="str">
         <f aca="false">IF(OR(ISNUMBER(SEARCH("D",B94)), ISNUMBER(SEARCH("D", C94))),"Cangi","Yelle")</f>
         <v>Yelle</v>
       </c>
@@ -60382,13 +60415,1018 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:O36"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="G36" activeCellId="0" sqref="G36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="23.01"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="F12" s="0" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="H33" s="0" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>263</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:N30"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="23.01"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>383</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="N13" s="0" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N15" s="0" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="N17" s="0" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="N18" s="0" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="N19" s="0" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>385</v>
+      </c>
+      <c r="N20" s="0" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>370</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>386</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AA32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="1" sqref="1:1 A15"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="4.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.65"/>
@@ -60474,8 +61512,8 @@
       </c>
     </row>
     <row r="2" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>380</v>
+      <c r="A2" s="6" t="s">
+        <v>387</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>175</v>
@@ -60541,6 +61579,7 @@
       </c>
     </row>
     <row r="3" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6"/>
       <c r="B3" s="1" t="n">
         <v>208</v>
       </c>
@@ -60595,13 +61634,14 @@
         <v>177</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="W3" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6"/>
       <c r="C4" s="1" t="s">
         <v>39</v>
       </c>
@@ -60660,6 +61700,7 @@
       </c>
     </row>
     <row r="5" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6"/>
       <c r="C5" s="1" t="s">
         <v>34</v>
       </c>
@@ -60721,6 +61762,7 @@
       </c>
     </row>
     <row r="6" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6"/>
       <c r="C6" s="1" t="s">
         <v>53</v>
       </c>
@@ -60782,6 +61824,7 @@
       </c>
     </row>
     <row r="7" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6"/>
       <c r="C7" s="1" t="s">
         <v>70</v>
       </c>
@@ -60838,7 +61881,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1"/>
+      <c r="A8" s="6"/>
       <c r="C8" s="0" t="s">
         <v>82</v>
       </c>
@@ -60901,7 +61944,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1"/>
+      <c r="A9" s="6"/>
       <c r="C9" s="0" t="s">
         <v>48</v>
       </c>
@@ -60958,7 +62001,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
+      <c r="A10" s="6"/>
       <c r="C10" s="0" t="s">
         <v>48</v>
       </c>
@@ -61015,7 +62058,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1"/>
+      <c r="A11" s="6"/>
       <c r="C11" s="0" t="s">
         <v>33</v>
       </c>
@@ -61065,7 +62108,7 @@
         <v>0</v>
       </c>
       <c r="T11" s="0" t="s">
-        <v>382</v>
+        <v>389</v>
       </c>
       <c r="U11" s="0" t="s">
         <v>37</v>
@@ -61075,7 +62118,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1"/>
+      <c r="A12" s="6"/>
       <c r="C12" s="0" t="s">
         <v>35</v>
       </c>
@@ -61125,7 +62168,7 @@
         <v>0</v>
       </c>
       <c r="T12" s="0" t="s">
-        <v>383</v>
+        <v>390</v>
       </c>
       <c r="U12" s="0" t="s">
         <v>50</v>
@@ -61135,7 +62178,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1"/>
+      <c r="A13" s="6"/>
       <c r="C13" s="0" t="s">
         <v>35</v>
       </c>
@@ -61191,14 +62234,14 @@
         <v>50</v>
       </c>
       <c r="V13" s="0" t="s">
-        <v>384</v>
+        <v>391</v>
       </c>
       <c r="W13" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1"/>
+      <c r="A14" s="6"/>
       <c r="B14" s="2" t="n">
         <f aca="false">ROW()-1</f>
         <v>13</v>
@@ -61267,7 +62310,7 @@
         <v>92</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="I15" s="0" t="n">
         <v>5</v>
@@ -61363,7 +62406,7 @@
         <v>0</v>
       </c>
       <c r="X16" s="0" t="s">
-        <v>386</v>
+        <v>393</v>
       </c>
       <c r="Y16" s="0" t="s">
         <v>108</v>
@@ -61426,7 +62469,7 @@
         <v>0</v>
       </c>
       <c r="X17" s="0" t="s">
-        <v>387</v>
+        <v>394</v>
       </c>
       <c r="Y17" s="0" t="s">
         <v>108</v>
@@ -61489,7 +62532,7 @@
         <v>298</v>
       </c>
       <c r="Y18" s="0" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
       <c r="AA18" s="1" t="s">
         <v>30</v>
@@ -61606,7 +62649,7 @@
         <v>0</v>
       </c>
       <c r="X20" s="0" t="s">
-        <v>389</v>
+        <v>396</v>
       </c>
       <c r="Y20" s="0" t="s">
         <v>108</v>
@@ -61729,7 +62772,7 @@
         <v>0</v>
       </c>
       <c r="X22" s="0" t="s">
-        <v>390</v>
+        <v>397</v>
       </c>
       <c r="Y22" s="0" t="s">
         <v>108</v>
@@ -61792,7 +62835,7 @@
         <v>0</v>
       </c>
       <c r="X23" s="0" t="s">
-        <v>391</v>
+        <v>398</v>
       </c>
       <c r="Y23" s="0" t="s">
         <v>108</v>
@@ -61855,7 +62898,7 @@
         <v>0</v>
       </c>
       <c r="X24" s="0" t="s">
-        <v>392</v>
+        <v>399</v>
       </c>
       <c r="Y24" s="0" t="s">
         <v>108</v>
@@ -61915,7 +62958,7 @@
         <v>0</v>
       </c>
       <c r="X25" s="0" t="s">
-        <v>393</v>
+        <v>400</v>
       </c>
       <c r="Y25" s="0" t="s">
         <v>108</v>
@@ -62095,7 +63138,7 @@
         <v>298</v>
       </c>
       <c r="Y28" s="0" t="s">
-        <v>394</v>
+        <v>401</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -62352,7 +63395,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -62360,17 +63403,17 @@
   <dimension ref="A1:Y46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A44" activeCellId="1" sqref="1:1 A44"/>
+      <selection pane="topLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
         <v>331</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>33</v>
@@ -62379,7 +63422,7 @@
         <v>290</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>-2</v>
@@ -62426,7 +63469,7 @@
         <v>332</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>35</v>
@@ -62435,7 +63478,7 @@
         <v>259</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>-2</v>
@@ -62482,7 +63525,7 @@
         <v>333</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>35</v>
@@ -62491,7 +63534,7 @@
         <v>290</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>34</v>
@@ -62541,7 +63584,7 @@
         <v>334</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>45</v>
@@ -62553,7 +63596,7 @@
         <v>27</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>-2</v>
@@ -62600,7 +63643,7 @@
         <v>335</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>45</v>
@@ -62612,7 +63655,7 @@
         <v>33</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>-2</v>
@@ -62659,7 +63702,7 @@
         <v>336</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>48</v>
@@ -62671,7 +63714,7 @@
         <v>32</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>-2</v>
@@ -62715,7 +63758,7 @@
         <v>337</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>64</v>
@@ -62724,7 +63767,7 @@
         <v>273</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>-2</v>
@@ -62768,7 +63811,7 @@
         <v>338</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>64</v>
@@ -62780,7 +63823,7 @@
         <v>32</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>-2</v>
@@ -62824,7 +63867,7 @@
         <v>339</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>64</v>
@@ -62836,7 +63879,7 @@
         <v>70</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>-2</v>
@@ -62880,7 +63923,7 @@
         <v>340</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>64</v>
@@ -62892,7 +63935,7 @@
         <v>33</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="G10" s="0" t="n">
         <v>-2</v>
@@ -62939,7 +63982,7 @@
         <v>341</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>64</v>
@@ -62951,7 +63994,7 @@
         <v>48</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="G11" s="0" t="n">
         <v>-2</v>
@@ -62995,13 +64038,13 @@
         <v>342</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>34</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>397</v>
+        <v>404</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>0</v>
@@ -63040,7 +64083,7 @@
         <v>0</v>
       </c>
       <c r="W12" s="0" t="s">
-        <v>398</v>
+        <v>405</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -63048,7 +64091,7 @@
         <v>343</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>34</v>
@@ -63057,7 +64100,7 @@
         <v>301</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="G13" s="0" t="n">
         <v>-2</v>
@@ -63104,7 +64147,7 @@
         <v>344</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>39</v>
@@ -63113,7 +64156,7 @@
         <v>275</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="G14" s="0" t="n">
         <v>-2</v>
@@ -63157,7 +64200,7 @@
         <v>345</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>39</v>
@@ -63166,7 +64209,7 @@
         <v>301</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>34</v>
@@ -63213,7 +64256,7 @@
         <v>346</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>80</v>
@@ -63222,7 +64265,7 @@
         <v>276</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="G16" s="0" t="n">
         <v>-2</v>
@@ -63266,7 +64309,7 @@
         <v>347</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>80</v>
@@ -63278,7 +64321,7 @@
         <v>53</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="G17" s="0" t="n">
         <v>-2</v>
@@ -63322,7 +64365,7 @@
         <v>348</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>80</v>
@@ -63331,7 +64374,7 @@
         <v>269</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>34</v>
@@ -63378,7 +64421,7 @@
         <v>349</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>55</v>
@@ -63390,7 +64433,7 @@
         <v>27</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="G19" s="0" t="n">
         <v>-2</v>
@@ -63434,7 +64477,7 @@
         <v>350</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>55</v>
@@ -63443,7 +64486,7 @@
         <v>296</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>34</v>
@@ -63490,7 +64533,7 @@
         <v>351</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>55</v>
@@ -63502,7 +64545,7 @@
         <v>59</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="G21" s="0" t="n">
         <v>-2</v>
@@ -63546,7 +64589,7 @@
         <v>352</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>55</v>
@@ -63558,7 +64601,7 @@
         <v>35</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="G22" s="0" t="n">
         <v>-2</v>
@@ -63602,7 +64645,7 @@
         <v>353</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>65</v>
@@ -63614,7 +64657,7 @@
         <v>32</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="G23" s="0" t="n">
         <v>-2</v>
@@ -63661,7 +64704,7 @@
         <v>354</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>65</v>
@@ -63670,7 +64713,7 @@
         <v>272</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>34</v>
@@ -63720,13 +64763,13 @@
         <v>355</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>65</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>397</v>
+        <v>404</v>
       </c>
       <c r="E25" s="0" t="s">
         <v>48</v>
@@ -63776,7 +64819,7 @@
         <v>356</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>122</v>
@@ -63788,7 +64831,7 @@
         <v>62</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="G26" s="0" t="n">
         <v>-2</v>
@@ -63835,7 +64878,7 @@
         <v>357</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>122</v>
@@ -63844,7 +64887,7 @@
         <v>281</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>34</v>
@@ -63894,7 +64937,7 @@
         <v>358</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>57</v>
@@ -63903,7 +64946,7 @@
         <v>278</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="G28" s="0" t="n">
         <v>-2</v>
@@ -63947,7 +64990,7 @@
         <v>359</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>57</v>
@@ -63959,7 +65002,7 @@
         <v>27</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="G29" s="0" t="n">
         <v>-2</v>
@@ -64003,7 +65046,7 @@
         <v>360</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>132</v>
@@ -64015,7 +65058,7 @@
         <v>32</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="G30" s="0" t="n">
         <v>-2</v>
@@ -64059,7 +65102,7 @@
         <v>361</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>132</v>
@@ -64071,7 +65114,7 @@
         <v>27</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="G31" s="0" t="n">
         <v>-2</v>
@@ -64115,7 +65158,7 @@
         <v>362</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>132</v>
@@ -64127,7 +65170,7 @@
         <v>62</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="G32" s="0" t="n">
         <v>-2</v>
@@ -64171,7 +65214,7 @@
         <v>363</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>132</v>
@@ -64183,7 +65226,7 @@
         <v>57</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="G33" s="0" t="n">
         <v>-2</v>
@@ -64227,7 +65270,7 @@
         <v>364</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>59</v>
@@ -64236,7 +65279,7 @@
         <v>370</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="F34" s="0" t="s">
         <v>34</v>
@@ -64286,7 +65329,7 @@
         <v>365</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>127</v>
@@ -64295,7 +65338,7 @@
         <v>310</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="F35" s="0" t="s">
         <v>34</v>
@@ -64345,7 +65388,7 @@
         <v>366</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>62</v>
@@ -64357,7 +65400,7 @@
         <v>32</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="G36" s="0" t="n">
         <v>-2</v>
@@ -64401,7 +65444,7 @@
         <v>367</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>62</v>
@@ -64413,7 +65456,7 @@
         <v>27</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="G37" s="0" t="n">
         <v>-2</v>
@@ -64457,7 +65500,7 @@
         <v>368</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>70</v>
@@ -64466,7 +65509,7 @@
         <v>283</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="G38" s="0" t="n">
         <v>-2</v>
@@ -64510,7 +65553,7 @@
         <v>369</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>70</v>
@@ -64522,7 +65565,7 @@
         <v>32</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="G39" s="0" t="n">
         <v>-2</v>
@@ -64566,7 +65609,7 @@
         <v>370</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>53</v>
@@ -64575,7 +65618,7 @@
         <v>279</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="F40" s="0" t="s">
         <v>34</v>
@@ -64625,13 +65668,13 @@
         <v>691</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>52</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="E41" s="0" t="n">
         <v>0</v>
@@ -64670,10 +65713,10 @@
         <v>0</v>
       </c>
       <c r="V41" s="0" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
       <c r="W41" s="0" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -64684,10 +65727,10 @@
         <v>275</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>397</v>
+        <v>404</v>
       </c>
       <c r="E42" s="0" t="s">
         <v>34</v>
@@ -64740,10 +65783,10 @@
         <v>301</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>397</v>
+        <v>404</v>
       </c>
       <c r="E43" s="0" t="n">
         <v>0</v>
@@ -64782,7 +65825,7 @@
         <v>0</v>
       </c>
       <c r="W43" s="0" t="s">
-        <v>401</v>
+        <v>408</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -64791,7 +65834,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>402</v>
+        <v>409</v>
       </c>
       <c r="C44" s="0" t="s">
         <v>39</v>
@@ -64836,7 +65879,7 @@
         <v>0</v>
       </c>
       <c r="W44" s="0" t="s">
-        <v>403</v>
+        <v>410</v>
       </c>
       <c r="Y44" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(SEARCH("D",B44)), ISNUMBER(SEARCH("D", C44))),"Cangi","Yelle")</f>
@@ -64849,7 +65892,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>402</v>
+        <v>409</v>
       </c>
       <c r="C45" s="0" t="s">
         <v>39</v>
@@ -64894,7 +65937,7 @@
         <v>0</v>
       </c>
       <c r="W45" s="0" t="s">
-        <v>403</v>
+        <v>410</v>
       </c>
       <c r="Y45" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(SEARCH("D",B45)), ISNUMBER(SEARCH("D", C45))),"Cangi","Yelle")</f>
@@ -64907,7 +65950,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>402</v>
+        <v>409</v>
       </c>
       <c r="C46" s="0" t="s">
         <v>39</v>
@@ -64952,7 +65995,7 @@
         <v>0</v>
       </c>
       <c r="W46" s="0" t="s">
-        <v>403</v>
+        <v>410</v>
       </c>
       <c r="Y46" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(SEARCH("D",B46)), ISNUMBER(SEARCH("D", C46))),"Cangi","Yelle")</f>

</xml_diff>

<commit_message>
Added some functions to the module, changed simulation to just use the default parameter file without asking, updated T function to use ion temps from Hanley 2022.
</commit_message>
<xml_diff>
--- a/REACTION_NETWORK.xlsx
+++ b/REACTION_NETWORK.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Neutral reactions" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8323" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8324" uniqueCount="416">
   <si>
     <t xml:space="preserve">R1</t>
   </si>
@@ -1116,6 +1116,30 @@
     <t xml:space="preserve">Npl</t>
   </si>
   <si>
+    <t xml:space="preserve">Fox1993</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Formatted to be the same as that used in Jane Fox’s 1993 nitrogen on Mars paper. Another option is Anicich2003: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">1.3E-10</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">NH4pl</t>
   </si>
   <si>
@@ -1277,7 +1301,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1299,6 +1323,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1387,11 +1417,11 @@
   </sheetPr>
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A259" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A259" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A279" activeCellId="0" sqref="A279"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53515625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.52734375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="19.61"/>
   </cols>
@@ -17346,16 +17376,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AG681"/>
+  <dimension ref="A1:AG1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A710" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A524" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D679" activeCellId="0" sqref="D679"/>
+      <selection pane="bottomLeft" activeCell="E541" activeCellId="0" sqref="E541"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53515625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.52734375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="11.4"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="26" min="20" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="14.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="35.84"/>
@@ -46041,7 +46072,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="451" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="451" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="1" t="s">
         <v>279</v>
       </c>
@@ -46063,11 +46094,11 @@
       <c r="G451" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q451" s="1" t="n">
-        <v>1.3E-010</v>
+      <c r="Q451" s="2" t="n">
+        <v>1.72E-009</v>
       </c>
       <c r="R451" s="1" t="n">
-        <v>0</v>
+        <v>-0.44</v>
       </c>
       <c r="S451" s="1" t="n">
         <v>0</v>
@@ -46097,7 +46128,10 @@
         <v>300</v>
       </c>
       <c r="AB451" s="1" t="s">
-        <v>358</v>
+        <v>363</v>
+      </c>
+      <c r="AC451" s="0" t="s">
+        <v>364</v>
       </c>
       <c r="AD451" s="1" t="s">
         <v>29</v>
@@ -46542,7 +46576,7 @@
         <v>79</v>
       </c>
       <c r="C459" s="1" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="D459" s="1" t="s">
         <v>31</v>
@@ -47224,7 +47258,7 @@
         <v>69</v>
       </c>
       <c r="C470" s="1" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="D470" s="1" t="s">
         <v>31</v>
@@ -47283,7 +47317,7 @@
         <v>34</v>
       </c>
       <c r="C471" s="1" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="D471" s="1" t="s">
         <v>32</v>
@@ -47345,7 +47379,7 @@
         <v>38</v>
       </c>
       <c r="C472" s="1" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="D472" s="1" t="s">
         <v>33</v>
@@ -47410,7 +47444,7 @@
         <v>79</v>
       </c>
       <c r="C473" s="1" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="D473" s="1" t="s">
         <v>52</v>
@@ -47469,7 +47503,7 @@
         <v>64</v>
       </c>
       <c r="C474" s="1" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="D474" s="1" t="s">
         <v>47</v>
@@ -50211,7 +50245,7 @@
         <v>72</v>
       </c>
       <c r="C519" s="1" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="D519" s="1" t="s">
         <v>33</v>
@@ -55132,10 +55166,10 @@
         <v>0</v>
       </c>
       <c r="AA596" s="1" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="AB596" s="1" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="AC596" s="1" t="s">
         <v>361</v>
@@ -55829,13 +55863,13 @@
         <v>0</v>
       </c>
       <c r="AA607" s="1" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="AB607" s="1" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="AC607" s="1" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="AD607" s="1" t="s">
         <v>29</v>
@@ -55894,7 +55928,7 @@
         <v>0</v>
       </c>
       <c r="AB608" s="1" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="AD608" s="1" t="s">
         <v>29</v>
@@ -55962,7 +55996,7 @@
         <v>324</v>
       </c>
       <c r="AB609" s="1" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="AD609" s="1" t="s">
         <v>29</v>
@@ -56083,7 +56117,7 @@
         <v>0</v>
       </c>
       <c r="AB611" s="1" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="AD611" s="1" t="s">
         <v>29</v>
@@ -56142,10 +56176,10 @@
         <v>0</v>
       </c>
       <c r="AB612" s="1" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="AC612" s="1" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="AD612" s="1" t="s">
         <v>29</v>
@@ -56204,10 +56238,10 @@
         <v>0</v>
       </c>
       <c r="AB613" s="1" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="AC613" s="1" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="AD613" s="1" t="s">
         <v>29</v>
@@ -56266,10 +56300,10 @@
         <v>0</v>
       </c>
       <c r="AA614" s="1" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="AB614" s="1" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="AC614" s="1" t="s">
         <v>361</v>
@@ -56334,7 +56368,7 @@
         <v>0</v>
       </c>
       <c r="AB615" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="AD615" s="1" t="s">
         <v>42</v>
@@ -56402,7 +56436,7 @@
         <v>0</v>
       </c>
       <c r="AB616" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="AD616" s="1" t="s">
         <v>42</v>
@@ -56470,7 +56504,7 @@
         <v>0</v>
       </c>
       <c r="AB617" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="AD617" s="1" t="s">
         <v>42</v>
@@ -56484,7 +56518,7 @@
         <v>51</v>
       </c>
       <c r="C618" s="1" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="D618" s="1" t="s">
         <v>31</v>
@@ -56532,7 +56566,7 @@
         <v>0</v>
       </c>
       <c r="AB618" s="1" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="AD618" s="1" t="s">
         <v>42</v>
@@ -56600,7 +56634,7 @@
         <v>0</v>
       </c>
       <c r="AB619" s="1" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="AD619" s="1" t="s">
         <v>42</v>
@@ -56662,7 +56696,7 @@
         <v>0</v>
       </c>
       <c r="AB620" s="1" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="AD620" s="1" t="s">
         <v>42</v>
@@ -57423,7 +57457,7 @@
         <v>300</v>
       </c>
       <c r="AB630" s="1" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="AD630" s="1" t="s">
         <v>29</v>
@@ -57491,7 +57525,7 @@
         <v>300</v>
       </c>
       <c r="AB631" s="1" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="AD631" s="1" t="s">
         <v>29</v>
@@ -57559,7 +57593,7 @@
         <v>300</v>
       </c>
       <c r="AB632" s="1" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="AD632" s="1" t="s">
         <v>29</v>
@@ -57627,7 +57661,7 @@
         <v>324</v>
       </c>
       <c r="AB633" s="1" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="AD633" s="1" t="s">
         <v>29</v>
@@ -57695,7 +57729,7 @@
         <v>0</v>
       </c>
       <c r="AB634" s="1" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="AD634" s="1" t="s">
         <v>29</v>
@@ -57760,7 +57794,7 @@
         <v>0</v>
       </c>
       <c r="AB635" s="1" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="AD635" s="1" t="s">
         <v>29</v>
@@ -57825,7 +57859,7 @@
         <v>0</v>
       </c>
       <c r="AB636" s="1" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="AD636" s="1" t="s">
         <v>29</v>
@@ -57890,7 +57924,7 @@
         <v>0</v>
       </c>
       <c r="AB637" s="1" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="AD637" s="1" t="s">
         <v>29</v>
@@ -57955,7 +57989,7 @@
         <v>0</v>
       </c>
       <c r="AA638" s="1" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="AB638" s="1" t="s">
         <v>36</v>
@@ -58026,7 +58060,7 @@
         <v>0</v>
       </c>
       <c r="AA639" s="1" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="AB639" s="1" t="s">
         <v>36</v>
@@ -58215,7 +58249,7 @@
         <v>300</v>
       </c>
       <c r="AB642" s="1" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="AD642" s="1" t="s">
         <v>42</v>
@@ -58283,7 +58317,7 @@
         <v>300</v>
       </c>
       <c r="AB643" s="1" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="AD643" s="1" t="s">
         <v>42</v>
@@ -58351,7 +58385,7 @@
         <v>300</v>
       </c>
       <c r="AB644" s="1" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="AD644" s="1" t="s">
         <v>29</v>
@@ -58413,7 +58447,7 @@
         <v>0</v>
       </c>
       <c r="AB645" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="AD645" s="1" t="s">
         <v>29</v>
@@ -58481,7 +58515,7 @@
         <v>0</v>
       </c>
       <c r="AB646" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="AD646" s="1" t="s">
         <v>29</v>
@@ -58543,7 +58577,7 @@
         <v>0</v>
       </c>
       <c r="AB647" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="AD647" s="1" t="s">
         <v>29</v>
@@ -58916,7 +58950,7 @@
         <v>0</v>
       </c>
       <c r="AA652" s="1" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="AB652" s="1" t="s">
         <v>41</v>
@@ -59238,7 +59272,7 @@
         <v>0</v>
       </c>
       <c r="AB657" s="1" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="AD657" s="1" t="s">
         <v>29</v>
@@ -59365,7 +59399,7 @@
         <v>0</v>
       </c>
       <c r="AB659" s="1" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="AD659" s="1" t="s">
         <v>29</v>
@@ -59566,7 +59600,7 @@
         <v>0</v>
       </c>
       <c r="AB662" s="1" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="AD662" s="1" t="s">
         <v>42</v>
@@ -59634,7 +59668,7 @@
         <v>0</v>
       </c>
       <c r="AB663" s="1" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="AD663" s="1" t="s">
         <v>42</v>
@@ -59693,7 +59727,7 @@
         <v>0</v>
       </c>
       <c r="AB664" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="AD664" s="1" t="s">
         <v>29</v>
@@ -59752,7 +59786,7 @@
         <v>0</v>
       </c>
       <c r="AB665" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="AD665" s="1" t="s">
         <v>29</v>
@@ -59811,7 +59845,7 @@
         <v>0</v>
       </c>
       <c r="AB666" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="AD666" s="1" t="s">
         <v>29</v>
@@ -59873,7 +59907,7 @@
         <v>360</v>
       </c>
       <c r="AC667" s="1" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="AD667" s="1" t="s">
         <v>29</v>
@@ -59935,7 +59969,7 @@
         <v>360</v>
       </c>
       <c r="AC668" s="1" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="AD668" s="1" t="s">
         <v>29</v>
@@ -60000,7 +60034,7 @@
         <v>0</v>
       </c>
       <c r="AA669" s="1" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="AB669" s="1" t="s">
         <v>36</v>
@@ -60068,7 +60102,7 @@
         <v>0</v>
       </c>
       <c r="AA670" s="1" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="AB670" s="1" t="s">
         <v>36</v>
@@ -60275,7 +60309,7 @@
         <v>324</v>
       </c>
       <c r="AB673" s="1" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="AD673" s="1" t="s">
         <v>29</v>
@@ -60399,7 +60433,7 @@
         <v>0</v>
       </c>
       <c r="AB675" s="1" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="AD675" s="1" t="s">
         <v>42</v>
@@ -60461,7 +60495,7 @@
         <v>0</v>
       </c>
       <c r="AB676" s="1" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="AD676" s="1" t="s">
         <v>42</v>
@@ -60579,10 +60613,10 @@
         <v>0</v>
       </c>
       <c r="AA678" s="4" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="AB678" s="4" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="AD678" s="4" t="s">
         <v>29</v>
@@ -60724,7 +60758,7 @@
         <v>324</v>
       </c>
       <c r="AB680" s="1" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="AD680" s="1" t="s">
         <v>29</v>
@@ -60792,6 +60826,7 @@
         <v>29</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -60814,7 +60849,7 @@
       <selection pane="topLeft" activeCell="M23" activeCellId="0" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53515625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.52734375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -60830,16 +60865,16 @@
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>246</v>
@@ -60892,7 +60927,7 @@
         <v>256</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>260</v>
@@ -60918,7 +60953,7 @@
         <v>31</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>260</v>
@@ -60944,7 +60979,7 @@
         <v>256</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>260</v>
@@ -60970,7 +61005,7 @@
         <v>256</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>290</v>
@@ -60996,7 +61031,7 @@
         <v>256</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>290</v>
@@ -61022,7 +61057,7 @@
         <v>256</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>290</v>
@@ -61048,7 +61083,7 @@
         <v>256</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>290</v>
@@ -61077,7 +61112,7 @@
         <v>256</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>290</v>
@@ -61106,7 +61141,7 @@
         <v>31</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>290</v>
@@ -61135,7 +61170,7 @@
         <v>256</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>290</v>
@@ -61164,7 +61199,7 @@
         <v>256</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>290</v>
@@ -61193,7 +61228,7 @@
         <v>256</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>290</v>
@@ -61219,7 +61254,7 @@
         <v>256</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>290</v>
@@ -61245,7 +61280,7 @@
         <v>256</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>290</v>
@@ -61274,7 +61309,7 @@
         <v>256</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>290</v>
@@ -61303,7 +61338,7 @@
         <v>31</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>290</v>
@@ -61332,7 +61367,7 @@
         <v>256</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>290</v>
@@ -61361,7 +61396,7 @@
         <v>256</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>290</v>
@@ -61390,7 +61425,7 @@
         <v>256</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>290</v>
@@ -61419,7 +61454,7 @@
         <v>256</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>290</v>
@@ -61445,7 +61480,7 @@
         <v>256</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>290</v>
@@ -61474,7 +61509,7 @@
         <v>256</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>290</v>
@@ -61500,7 +61535,7 @@
         <v>256</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>290</v>
@@ -61526,7 +61561,7 @@
         <v>256</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>260</v>
@@ -61552,7 +61587,7 @@
         <v>256</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>260</v>
@@ -61578,7 +61613,7 @@
         <v>256</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>260</v>
@@ -61604,7 +61639,7 @@
         <v>256</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>290</v>
@@ -61630,7 +61665,7 @@
         <v>256</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>290</v>
@@ -61656,7 +61691,7 @@
         <v>31</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>290</v>
@@ -61682,7 +61717,7 @@
         <v>256</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>290</v>
@@ -61708,7 +61743,7 @@
         <v>256</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>290</v>
@@ -61734,7 +61769,7 @@
         <v>256</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>290</v>
@@ -61763,7 +61798,7 @@
         <v>256</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>290</v>
@@ -61792,7 +61827,7 @@
         <v>256</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>290</v>
@@ -61821,7 +61856,7 @@
         <v>256</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>290</v>
@@ -61853,13 +61888,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T37"/>
+  <dimension ref="A1:T44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="Q24" activeCellId="0" sqref="Q24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53515625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.52734375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -61875,16 +61910,16 @@
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>246</v>
@@ -61937,7 +61972,7 @@
         <v>256</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>260</v>
@@ -61963,7 +61998,7 @@
         <v>256</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>260</v>
@@ -61989,7 +62024,7 @@
         <v>256</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>260</v>
@@ -62015,7 +62050,7 @@
         <v>256</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>260</v>
@@ -62032,7 +62067,7 @@
         <v>63</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>256</v>
@@ -62041,7 +62076,7 @@
         <v>256</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>260</v>
@@ -62067,7 +62102,7 @@
         <v>256</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>260</v>
@@ -62093,7 +62128,7 @@
         <v>256</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>260</v>
@@ -62110,7 +62145,7 @@
         <v>63</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>69</v>
@@ -62119,7 +62154,7 @@
         <v>256</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>260</v>
@@ -62145,7 +62180,7 @@
         <v>256</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>260</v>
@@ -62171,7 +62206,7 @@
         <v>256</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>260</v>
@@ -62183,7 +62218,7 @@
         <v>286</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62200,7 +62235,7 @@
         <v>256</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>260</v>
@@ -62212,7 +62247,7 @@
         <v>0</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62229,7 +62264,7 @@
         <v>256</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>260</v>
@@ -62255,7 +62290,7 @@
         <v>256</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>260</v>
@@ -62270,7 +62305,7 @@
         <v>260</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62287,7 +62322,7 @@
         <v>256</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>260</v>
@@ -62305,7 +62340,7 @@
         <v>0.5</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62322,7 +62357,7 @@
         <v>256</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>260</v>
@@ -62340,7 +62375,7 @@
         <v>0.5</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62357,7 +62392,7 @@
         <v>256</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>260</v>
@@ -62383,7 +62418,7 @@
         <v>256</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>260</v>
@@ -62395,7 +62430,7 @@
         <v>0</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62412,7 +62447,7 @@
         <v>256</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>260</v>
@@ -62427,7 +62462,7 @@
         <v>260</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62444,7 +62479,7 @@
         <v>256</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>260</v>
@@ -62459,7 +62494,7 @@
         <v>260</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62467,7 +62502,7 @@
         <v>75</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>256</v>
@@ -62476,7 +62511,7 @@
         <v>256</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>260</v>
@@ -62488,7 +62523,7 @@
         <v>0</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62505,7 +62540,7 @@
         <v>256</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>260</v>
@@ -62531,7 +62566,7 @@
         <v>256</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>260</v>
@@ -62557,7 +62592,7 @@
         <v>256</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>260</v>
@@ -62572,7 +62607,7 @@
         <v>0.5</v>
       </c>
       <c r="T24" s="1" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62589,7 +62624,7 @@
         <v>256</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>260</v>
@@ -62604,7 +62639,7 @@
         <v>0.5</v>
       </c>
       <c r="T25" s="1" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62621,7 +62656,7 @@
         <v>256</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>260</v>
@@ -62639,7 +62674,7 @@
         <v>0.5</v>
       </c>
       <c r="T26" s="1" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62656,7 +62691,7 @@
         <v>256</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>260</v>
@@ -62674,7 +62709,7 @@
         <v>0.5</v>
       </c>
       <c r="T27" s="1" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62691,7 +62726,7 @@
         <v>256</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>260</v>
@@ -62706,7 +62741,7 @@
         <v>260</v>
       </c>
       <c r="T28" s="1" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62723,7 +62758,7 @@
         <v>256</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>260</v>
@@ -62749,7 +62784,7 @@
         <v>256</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>260</v>
@@ -62775,7 +62810,7 @@
         <v>256</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>260</v>
@@ -62801,7 +62836,7 @@
         <v>256</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>260</v>
@@ -62827,7 +62862,7 @@
         <v>256</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>260</v>
@@ -62853,7 +62888,7 @@
         <v>256</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>260</v>
@@ -62879,7 +62914,7 @@
         <v>256</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>260</v>
@@ -62896,7 +62931,7 @@
         <v>85</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>256</v>
@@ -62905,7 +62940,7 @@
         <v>256</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>260</v>
@@ -62947,7 +62982,7 @@
       <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53515625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.52734375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -63123,7 +63158,7 @@
         <v>176</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="U3" s="1" t="s">
         <v>29</v>
@@ -63568,7 +63603,7 @@
         <v>0</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="S11" s="1" t="s">
         <v>36</v>
@@ -63627,7 +63662,7 @@
         <v>0</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="S12" s="1" t="s">
         <v>49</v>
@@ -63692,7 +63727,7 @@
         <v>49</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="U13" s="1" t="s">
         <v>29</v>
@@ -63753,7 +63788,7 @@
         <v>91</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="G15" s="1" t="n">
         <v>5</v>
@@ -64647,10 +64682,10 @@
         <v>0</v>
       </c>
       <c r="T33" s="0" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="W33" s="1" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="Y33" s="1" t="s">
         <v>42</v>
@@ -64679,14 +64714,14 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53515625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.52734375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>32</v>
@@ -64695,7 +64730,7 @@
         <v>289</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -64703,7 +64738,7 @@
         <v>332</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>34</v>
@@ -64712,7 +64747,7 @@
         <v>265</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -64720,7 +64755,7 @@
         <v>333</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>34</v>
@@ -64729,7 +64764,7 @@
         <v>289</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -64737,7 +64772,7 @@
         <v>334</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>44</v>
@@ -64754,7 +64789,7 @@
         <v>335</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>44</v>
@@ -64771,7 +64806,7 @@
         <v>336</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>47</v>
@@ -64788,7 +64823,7 @@
         <v>337</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>63</v>
@@ -64797,7 +64832,7 @@
         <v>275</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -64805,7 +64840,7 @@
         <v>338</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>63</v>
@@ -64822,7 +64857,7 @@
         <v>339</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>63</v>
@@ -64839,7 +64874,7 @@
         <v>340</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>63</v>
@@ -64856,7 +64891,7 @@
         <v>341</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>63</v>
@@ -64873,13 +64908,13 @@
         <v>342</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="E12" s="1" t="n">
         <v>0</v>
@@ -64890,7 +64925,7 @@
         <v>343</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>33</v>
@@ -64899,7 +64934,7 @@
         <v>301</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -64907,7 +64942,7 @@
         <v>344</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>38</v>
@@ -64916,7 +64951,7 @@
         <v>276</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -64924,7 +64959,7 @@
         <v>345</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>38</v>
@@ -64933,7 +64968,7 @@
         <v>301</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -64941,7 +64976,7 @@
         <v>346</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>79</v>
@@ -64950,7 +64985,7 @@
         <v>277</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -64958,7 +64993,7 @@
         <v>347</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>79</v>
@@ -64975,7 +65010,7 @@
         <v>348</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>79</v>
@@ -64984,7 +65019,7 @@
         <v>271</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -64992,7 +65027,7 @@
         <v>349</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>54</v>
@@ -65009,7 +65044,7 @@
         <v>350</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>54</v>
@@ -65018,7 +65053,7 @@
         <v>296</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -65026,7 +65061,7 @@
         <v>351</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>54</v>
@@ -65043,7 +65078,7 @@
         <v>352</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>54</v>
@@ -65060,7 +65095,7 @@
         <v>353</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>64</v>
@@ -65077,7 +65112,7 @@
         <v>354</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>64</v>
@@ -65086,7 +65121,7 @@
         <v>274</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -65094,13 +65129,13 @@
         <v>355</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>64</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>47</v>
@@ -65111,7 +65146,7 @@
         <v>356</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>121</v>
@@ -65128,7 +65163,7 @@
         <v>357</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>121</v>
@@ -65137,7 +65172,7 @@
         <v>282</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -65145,7 +65180,7 @@
         <v>358</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>56</v>
@@ -65154,7 +65189,7 @@
         <v>279</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -65162,7 +65197,7 @@
         <v>359</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>56</v>
@@ -65179,7 +65214,7 @@
         <v>360</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>131</v>
@@ -65196,7 +65231,7 @@
         <v>361</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>131</v>
@@ -65213,7 +65248,7 @@
         <v>362</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>131</v>
@@ -65230,7 +65265,7 @@
         <v>363</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>131</v>
@@ -65247,7 +65282,7 @@
         <v>364</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>58</v>
@@ -65256,7 +65291,7 @@
         <v>362</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -65264,7 +65299,7 @@
         <v>365</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>126</v>
@@ -65273,7 +65308,7 @@
         <v>310</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -65281,7 +65316,7 @@
         <v>366</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>61</v>
@@ -65298,7 +65333,7 @@
         <v>367</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>61</v>
@@ -65315,7 +65350,7 @@
         <v>368</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>69</v>
@@ -65324,7 +65359,7 @@
         <v>284</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -65332,7 +65367,7 @@
         <v>369</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>69</v>
@@ -65349,7 +65384,7 @@
         <v>370</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>52</v>
@@ -65358,7 +65393,7 @@
         <v>280</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -65366,13 +65401,13 @@
         <v>691</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="E41" s="1" t="n">
         <v>0</v>
@@ -65386,10 +65421,10 @@
         <v>276</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>33</v>
@@ -65403,10 +65438,10 @@
         <v>301</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="E43" s="1" t="n">
         <v>0</v>
@@ -65417,7 +65452,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>38</v>
@@ -65434,7 +65469,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>38</v>
@@ -65451,7 +65486,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
Updates to photochemistry module, removal of unneeded files
</commit_message>
<xml_diff>
--- a/REACTION_NETWORK.xlsx
+++ b/REACTION_NETWORK.xlsx
@@ -5,15 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Neutral reactions" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Ion reactions" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Photodissociation" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Photoionization" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Unused neutrals" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Unused ion reactions" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8324" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7960" uniqueCount="404">
   <si>
     <t xml:space="preserve">R1</t>
   </si>
@@ -1119,25 +1117,7 @@
     <t xml:space="preserve">Fox1993</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Formatted to be the same as that used in Jane Fox’s 1993 nitrogen on Mars paper. Another option is Anicich2003: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">1.3E-10</t>
-    </r>
+    <t xml:space="preserve">Formatted to be the same as that used in Jane Fox’s 1993 nitrogen on Mars paper. Another option is Anicich2003: 1.3E-10</t>
   </si>
   <si>
     <t xml:space="preserve">NH4pl</t>
@@ -1256,42 +1236,6 @@
   <si>
     <t xml:space="preserve">O3pl</t>
   </si>
-  <si>
-    <t xml:space="preserve">Atkinson89, Sander15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">300-14700</t>
-  </si>
-  <si>
-    <t xml:space="preserve">200-1000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Approximated Fc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N2O5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rate from Burkholder but it doesn’t seem to produce a stable atmo…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Burkholder 2020. 1.3?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">331</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hepl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">He</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HeHpl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O2Dpl</t>
-  </si>
 </sst>
 </file>
 
@@ -1301,7 +1245,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1323,12 +1267,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1421,7 +1359,7 @@
       <selection pane="topLeft" activeCell="A279" activeCellId="0" sqref="A279"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.52734375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="19.61"/>
   </cols>
@@ -17378,13 +17316,13 @@
   </sheetPr>
   <dimension ref="A1:AG1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A524" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="E541" activeCellId="0" sqref="E541"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.52734375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="11.4"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="26" min="20" style="0" width="10.58"/>
@@ -60849,7 +60787,7 @@
       <selection pane="topLeft" activeCell="M23" activeCellId="0" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.52734375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -61890,11 +61828,11 @@
   </sheetPr>
   <dimension ref="A1:T44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="Q24" activeCellId="0" sqref="Q24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.52734375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -62969,2542 +62907,4 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:Y35"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.52734375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="H2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1" t="n">
-        <v>900</v>
-      </c>
-      <c r="K2" s="1" t="n">
-        <v>5.21E-035</v>
-      </c>
-      <c r="L2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" s="1" t="n">
-        <v>900</v>
-      </c>
-      <c r="N2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="H3" s="1" t="n">
-        <v>2.8E-012</v>
-      </c>
-      <c r="I3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" s="1" t="n">
-        <v>5.29E-028</v>
-      </c>
-      <c r="L3" s="1" t="n">
-        <v>-2.4</v>
-      </c>
-      <c r="M3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="1" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H4" s="1" t="n">
-        <v>6.44E-020</v>
-      </c>
-      <c r="I4" s="1" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="J4" s="1" t="n">
-        <v>-3150</v>
-      </c>
-      <c r="K4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="H5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" s="1" t="n">
-        <v>-1</v>
-      </c>
-      <c r="J5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="1" t="n">
-        <v>1.8E-030</v>
-      </c>
-      <c r="L5" s="1" t="n">
-        <v>-1</v>
-      </c>
-      <c r="M5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="1" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="H6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I6" s="1" t="n">
-        <v>-2</v>
-      </c>
-      <c r="J6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" s="1" t="n">
-        <v>6.1E-026</v>
-      </c>
-      <c r="L6" s="1" t="n">
-        <v>-2</v>
-      </c>
-      <c r="M6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" s="1" t="n">
-        <v>6E-016</v>
-      </c>
-      <c r="O6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="1" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H7" s="1" t="n">
-        <v>2.4E-011</v>
-      </c>
-      <c r="I7" s="1" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="J7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="1" t="n">
-        <v>7.31E-029</v>
-      </c>
-      <c r="L7" s="1" t="n">
-        <v>-1.3</v>
-      </c>
-      <c r="M7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="H8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" s="1" t="n">
-        <v>920</v>
-      </c>
-      <c r="K8" s="1" t="n">
-        <v>2.1E-033</v>
-      </c>
-      <c r="L8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M8" s="1" t="n">
-        <v>920</v>
-      </c>
-      <c r="N8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H9" s="1" t="n">
-        <v>1.5E-013</v>
-      </c>
-      <c r="I9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E10" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H10" s="1" t="n">
-        <v>6.62E-016</v>
-      </c>
-      <c r="I10" s="1" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="J10" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" s="1" t="n">
-        <v>1.77E-030</v>
-      </c>
-      <c r="L10" s="1" t="n">
-        <v>-1</v>
-      </c>
-      <c r="M10" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N10" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P10" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="U10" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H11" s="1" t="n">
-        <v>6.93E-020</v>
-      </c>
-      <c r="I11" s="1" t="n">
-        <v>0.37</v>
-      </c>
-      <c r="J11" s="1" t="n">
-        <v>-51</v>
-      </c>
-      <c r="K11" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L11" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M11" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N11" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O11" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P11" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U11" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H12" s="1" t="n">
-        <v>2.9E-010</v>
-      </c>
-      <c r="I12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" s="1" t="n">
-        <v>-1670</v>
-      </c>
-      <c r="K12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="U12" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="H13" s="1" t="n">
-        <v>8.5E-011</v>
-      </c>
-      <c r="I13" s="1" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="J13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" s="1" t="n">
-        <v>4.7E-026</v>
-      </c>
-      <c r="L13" s="1" t="n">
-        <v>-1.6</v>
-      </c>
-      <c r="M13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="1" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="S13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="T13" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="U13" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H14" s="1" t="n">
-        <v>1.62847E-006</v>
-      </c>
-      <c r="I14" s="1" t="n">
-        <v>6.1</v>
-      </c>
-      <c r="J14" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" s="1" t="n">
-        <v>4.89574E-015</v>
-      </c>
-      <c r="L14" s="1" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="M14" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N14" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O14" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P14" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="G15" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H15" s="1" t="n">
-        <v>9.04E-013</v>
-      </c>
-      <c r="I15" s="1" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="J15" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K15" s="1" t="n">
-        <v>6.48E-023</v>
-      </c>
-      <c r="L15" s="1" t="n">
-        <v>-3</v>
-      </c>
-      <c r="M15" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N15" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O15" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P15" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H16" s="1" t="n">
-        <v>7.8E-011</v>
-      </c>
-      <c r="I16" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" s="1" t="n">
-        <v>-3400</v>
-      </c>
-      <c r="K16" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L16" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M16" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N16" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O16" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P16" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G17" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H17" s="1" t="n">
-        <v>1.3E-012</v>
-      </c>
-      <c r="I17" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J17" s="1" t="n">
-        <v>380</v>
-      </c>
-      <c r="K17" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L17" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M17" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N17" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O17" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P17" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G18" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H18" s="1" t="n">
-        <v>1.35E-017</v>
-      </c>
-      <c r="I18" s="1" t="n">
-        <v>1.89</v>
-      </c>
-      <c r="J18" s="1" t="n">
-        <v>-1940</v>
-      </c>
-      <c r="K18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G19" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H19" s="1" t="n">
-        <v>2.01E-011</v>
-      </c>
-      <c r="I19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J19" s="1" t="n">
-        <v>-3000</v>
-      </c>
-      <c r="K19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G20" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H20" s="1" t="n">
-        <v>1.8E-011</v>
-      </c>
-      <c r="I20" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J20" s="1" t="n">
-        <v>-390</v>
-      </c>
-      <c r="K20" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L20" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M20" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N20" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O20" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P20" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G21" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H21" s="1" t="n">
-        <v>3.5E-012</v>
-      </c>
-      <c r="I21" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J21" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K21" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L21" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M21" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N21" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O21" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P21" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G22" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H22" s="1" t="n">
-        <v>1.5E-011</v>
-      </c>
-      <c r="I22" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J22" s="1" t="n">
-        <v>170</v>
-      </c>
-      <c r="K22" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L22" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M22" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N22" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O22" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P22" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G23" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H23" s="1" t="n">
-        <v>4.5E-014</v>
-      </c>
-      <c r="I23" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J23" s="1" t="n">
-        <v>-1260</v>
-      </c>
-      <c r="K23" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L23" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M23" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N23" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O23" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P23" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G24" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H24" s="1" t="n">
-        <v>8.5E-013</v>
-      </c>
-      <c r="I24" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J24" s="1" t="n">
-        <v>-2450</v>
-      </c>
-      <c r="K24" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L24" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M24" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N24" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O24" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P24" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G25" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H25" s="1" t="n">
-        <v>1E-011</v>
-      </c>
-      <c r="I25" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J25" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K25" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L25" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M25" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N25" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O25" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P25" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G26" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H26" s="1" t="n">
-        <v>2.2E-011</v>
-      </c>
-      <c r="I26" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J26" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K26" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L26" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M26" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N26" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O26" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P26" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G27" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H27" s="1" t="n">
-        <v>1.8E-012</v>
-      </c>
-      <c r="I27" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J27" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K27" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L27" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M27" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N27" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O27" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P27" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G28" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H28" s="1" t="n">
-        <v>2.16E-011</v>
-      </c>
-      <c r="I28" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J28" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K28" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L28" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M28" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N28" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O28" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P28" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G29" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H29" s="1" t="n">
-        <v>1.16E-009</v>
-      </c>
-      <c r="I29" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J29" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K29" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L29" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M29" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N29" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O29" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P29" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G30" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H30" s="1" t="n">
-        <v>1.7E-011</v>
-      </c>
-      <c r="I30" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J30" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K30" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L30" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M30" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N30" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O30" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P30" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G31" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H31" s="1" t="n">
-        <v>6.29E-018</v>
-      </c>
-      <c r="I31" s="1" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="J31" s="1" t="n">
-        <v>70</v>
-      </c>
-      <c r="K31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G32" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H32" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I32" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J32" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K32" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L32" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M32" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N32" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O32" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P32" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q32" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G33" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H33" s="1" t="n">
-        <v>2.6E-011</v>
-      </c>
-      <c r="I33" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J33" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K33" s="1" t="n">
-        <v>2.691E-028</v>
-      </c>
-      <c r="L33" s="1" t="n">
-        <v>-1</v>
-      </c>
-      <c r="M33" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N33" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O33" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P33" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q33" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T33" s="0" t="s">
-        <v>409</v>
-      </c>
-      <c r="W33" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="Y33" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:E46"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.52734375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>332</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>333</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>334</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>335</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <v>336</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
-        <v>337</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
-        <v>338</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
-        <v>339</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
-        <v>340</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
-        <v>341</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
-        <v>342</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="E12" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
-        <v>343</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
-        <v>344</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
-        <v>345</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
-        <v>346</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
-        <v>347</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
-        <v>348</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
-        <v>349</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
-        <v>350</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
-        <v>351</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="n">
-        <v>352</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
-        <v>353</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
-        <v>354</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
-        <v>355</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="n">
-        <v>356</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="n">
-        <v>357</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
-        <v>358</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="n">
-        <v>359</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="n">
-        <v>360</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="n">
-        <v>361</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="n">
-        <v>362</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="n">
-        <v>363</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="n">
-        <v>364</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="n">
-        <v>365</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="n">
-        <v>366</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="n">
-        <v>367</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="n">
-        <v>368</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="n">
-        <v>369</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="n">
-        <v>370</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="n">
-        <v>691</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="E41" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="n">
-        <v>222</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="n">
-        <v>422</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="E43" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="n">
-        <v>43</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="n">
-        <v>44</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update files, prepare for submission of paper 2.
</commit_message>
<xml_diff>
--- a/REACTION_NETWORK.xlsx
+++ b/REACTION_NETWORK.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Neutral reactions" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7960" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7962" uniqueCount="404">
   <si>
     <t xml:space="preserve">R1</t>
   </si>
@@ -1359,7 +1359,7 @@
       <selection pane="topLeft" activeCell="A279" activeCellId="0" sqref="A279"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="19.61"/>
   </cols>
@@ -17316,18 +17316,18 @@
   </sheetPr>
   <dimension ref="A1:AG1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A524" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E541" activeCellId="0" sqref="E541"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="AC173" activeCellId="0" sqref="AC173"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="11.4"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="26" min="20" style="0" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="26" min="20" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="14.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="35.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="69.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="15.83"/>
   </cols>
   <sheetData>
@@ -28243,6 +28243,9 @@
       <c r="H173" s="1" t="s">
         <v>290</v>
       </c>
+      <c r="J173" s="0" t="s">
+        <v>290</v>
+      </c>
       <c r="P173" s="1" t="n">
         <v>0.87</v>
       </c>
@@ -41370,6 +41373,9 @@
         <v>-0.13</v>
       </c>
       <c r="H377" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="I377" s="0" t="s">
         <v>290</v>
       </c>
       <c r="Q377" s="1" t="n">
@@ -60787,7 +60793,7 @@
       <selection pane="topLeft" activeCell="M23" activeCellId="0" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -61828,11 +61834,11 @@
   </sheetPr>
   <dimension ref="A1:T44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="Q24" activeCellId="0" sqref="Q24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
- Update model to allow turning ambipolar and molecular diffusion on and off in order to reproduce results of past studies. - Update content of some notebooks that were previously used for generating model-relevant input but no longer are. - Add an analysis function called plot_directional_flux which does what it suggests, per request of a coauthor. - Add plotting functions to show net volume change at a given atmospheric layer and the reaction rate of a given reaction as a function of altitude. - Make some cosmetic changes to code formatting - Fix an error in the branching ratio for HCO+ dissociative recombination which resulted in an underestimate of the importance by 10% or so. - Delete some no longer necessary lines that were previously commented out in converge_new_file.
</commit_message>
<xml_diff>
--- a/REACTION_NETWORK.xlsx
+++ b/REACTION_NETWORK.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Neutral reactions" sheetId="1" state="visible" r:id="rId2"/>
@@ -2214,11 +2214,11 @@
   </sheetPr>
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A166" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A186" activeCellId="0" sqref="A186"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A280" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A186" activeCellId="1" sqref="618:620 A186"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.56640625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -18011,13 +18011,16 @@
   </sheetPr>
   <dimension ref="A1:AF684"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A624" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="AD654" activeCellId="0" sqref="AD654"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A606" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
+      <selection pane="bottomLeft" activeCell="O620" activeCellId="0" sqref="618:620"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.56640625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="16.97"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -58531,7 +58534,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="649" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="649" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A649" s="1" t="s">
         <v>50</v>
       </c>
@@ -58560,7 +58563,7 @@
         <v>0.92</v>
       </c>
       <c r="S649" s="1" t="n">
-        <v>1.06E-005</v>
+        <v>1.15E-007</v>
       </c>
       <c r="T649" s="1" t="n">
         <v>-0.64</v>
@@ -58596,7 +58599,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="650" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="650" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A650" s="1" t="s">
         <v>50</v>
       </c>
@@ -58619,7 +58622,7 @@
         <v>0.07</v>
       </c>
       <c r="S650" s="1" t="n">
-        <v>8.08E-007</v>
+        <v>1.15E-007</v>
       </c>
       <c r="T650" s="1" t="n">
         <v>-0.64</v>
@@ -60788,10 +60791,10 @@
   <dimension ref="A1:V36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="1" sqref="618:620 A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.56640625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -61877,10 +61880,10 @@
   <dimension ref="A1:V36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="618:620 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.56640625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>